<commit_message>
Clone and Merge Object
Clone and Merge Object
</commit_message>
<xml_diff>
--- a/React B10 G1/React_B10_G1(1).xlsx
+++ b/React B10 G1/React_B10_G1(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashish\React\javascript\React B10 G1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654C4B8F-6832-437D-BE72-695EF9FFEBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E0B5A4-05E9-4351-B845-8D989C17C45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="12">
   <si>
     <t>Student Name</t>
   </si>
@@ -629,7 +629,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -669,7 +669,9 @@
       <c r="J1" s="4">
         <v>45301</v>
       </c>
-      <c r="K1" s="5"/>
+      <c r="K1" s="4">
+        <v>45302</v>
+      </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -711,7 +713,9 @@
       <c r="J2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="7"/>
+      <c r="K2" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -753,7 +757,9 @@
       <c r="J3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="7"/>
+      <c r="K3" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
@@ -795,7 +801,9 @@
       <c r="J4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
@@ -837,7 +845,9 @@
       <c r="J5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -879,7 +889,9 @@
       <c r="J6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="7"/>
+      <c r="K6" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -892,7 +904,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:F6 H2:J6" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:F6 H2:K6" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>